<commit_message>
updated role matrix, created roles, created files to rebuild database
</commit_message>
<xml_diff>
--- a/role_matrix.xlsx
+++ b/role_matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Desktop\DP-react\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Desktop\DP-react\diplo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0187C7AB-C147-4B61-B1EB-BAB4A1D8347E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12570513-D381-4CDF-8A91-70D42F9640EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8777963-E81B-4BA9-8F52-12284E87A50A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8777963-E81B-4BA9-8F52-12284E87A50A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="26">
   <si>
-    <t>u_default_connection</t>
-  </si>
-  <si>
     <t>student</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>members</t>
   </si>
   <si>
-    <t>admin has SUPERUSER role and therefore has all privileges</t>
-  </si>
-  <si>
     <t>bookings</t>
   </si>
   <si>
@@ -116,6 +110,12 @@
   </si>
   <si>
     <t>u_executioner</t>
+  </si>
+  <si>
+    <t>u_connection</t>
+  </si>
+  <si>
+    <t>admin will have full privileges except superuser and createrole options</t>
   </si>
 </sst>
 </file>
@@ -687,13 +687,13 @@
   <dimension ref="B1:BB12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP6" sqref="AP6"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
     <col min="3" max="54" width="2.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -701,79 +701,79 @@
     <row r="2" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B2" s="19"/>
       <c r="C2" s="29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
       <c r="G2" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
       <c r="N2" s="24"/>
       <c r="O2" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
       <c r="S2" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T2" s="23"/>
       <c r="U2" s="23"/>
       <c r="V2" s="24"/>
       <c r="W2" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X2" s="23"/>
       <c r="Y2" s="23"/>
       <c r="Z2" s="24"/>
       <c r="AA2" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB2" s="23"/>
       <c r="AC2" s="23"/>
       <c r="AD2" s="23"/>
       <c r="AE2" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AF2" s="23"/>
       <c r="AG2" s="23"/>
       <c r="AH2" s="24"/>
       <c r="AI2" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ2" s="23"/>
       <c r="AK2" s="23"/>
       <c r="AL2" s="23"/>
       <c r="AM2" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AN2" s="23"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="24"/>
       <c r="AQ2" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AR2" s="14"/>
       <c r="AS2" s="14"/>
       <c r="AT2" s="14"/>
       <c r="AU2" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AV2" s="14"/>
       <c r="AW2" s="14"/>
       <c r="AX2" s="15"/>
       <c r="AY2" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AZ2" s="14"/>
       <c r="BA2" s="14"/>
@@ -837,976 +837,976 @@
     <row r="4" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="21"/>
       <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="K4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="O4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="S4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="V4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="W4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="AA4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="AE4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AH4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AH4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="AI4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AL4" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="AM4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AO4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AP4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AP4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="AQ4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AR4" s="4" t="s">
+      <c r="AS4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AS4" s="4" t="s">
+      <c r="AT4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AT4" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="AU4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AV4" s="4" t="s">
+      <c r="AW4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AW4" s="4" t="s">
+      <c r="AX4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AX4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="AY4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AZ4" s="4" t="s">
+      <c r="BA4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="BA4" s="4" t="s">
+      <c r="BB4" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="BB4" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="V5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Y5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Z5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AE5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AF5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AG5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AI5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AJ5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AK5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AN5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AO5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AP5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AQ5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AR5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AT5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AU5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AW5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AX5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AY5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AZ5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BA5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BB5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AG6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AI6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AJ6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AK6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AN6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AO6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AP6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AQ6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AR6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AS6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AT6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AU6" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AW6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AX6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AY6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AZ6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BA6" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BB6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="V7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Y7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Z7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AE7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AF7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AG7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AI7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AJ7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AK7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AN7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AO7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AP7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AQ7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AR7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AS7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AT7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AU7" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AV7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AW7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AX7" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AY7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AZ7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BA7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BB7" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Y8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AB8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AE8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AF8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AG8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AI8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AJ8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AK8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AN8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AO8" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AP8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AQ8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AR8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AS8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AT8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AU8" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AV8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AW8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AX8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AY8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AZ8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BA8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BB8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AF9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AG9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AI9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AJ9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AK9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AL9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AM9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AN9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AO9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AP9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AQ9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AR9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AS9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AT9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AU9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AV9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AW9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AX9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AY9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AZ9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BA9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BB9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:54" x14ac:dyDescent="0.35">
       <c r="B12" s="12"/>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated database schema, created proposal for AST structure
</commit_message>
<xml_diff>
--- a/role_matrix.xlsx
+++ b/role_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Desktop\DP-react\diplo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12570513-D381-4CDF-8A91-70D42F9640EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6376D08-FBEB-4C27-9C95-818CF6A94B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8777963-E81B-4BA9-8F52-12284E87A50A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F8777963-E81B-4BA9-8F52-12284E87A50A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="24">
   <si>
     <t>student</t>
   </si>
@@ -66,13 +66,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>tokens</t>
-  </si>
-  <si>
-    <t>users to
-chapters</t>
   </si>
   <si>
     <t>users to
@@ -287,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -366,9 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +666,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -684,54 +674,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8353F37-9CE2-4E62-9A0C-B7CD2B1A2A97}">
-  <dimension ref="B1:BB12"/>
+  <dimension ref="B1:AT12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.7265625" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="54" width="2.6328125" customWidth="1"/>
+    <col min="3" max="46" width="2.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:54" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B2" s="19"/>
-      <c r="C2" s="29" t="s">
-        <v>10</v>
+      <c r="C2" s="23" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="23" t="s">
-        <v>7</v>
+      <c r="F2" s="23"/>
+      <c r="G2" s="27" t="s">
+        <v>8</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="27" t="s">
-        <v>8</v>
+      <c r="J2" s="24"/>
+      <c r="K2" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="22" t="s">
-        <v>12</v>
+      <c r="N2" s="23"/>
+      <c r="O2" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="27" t="s">
-        <v>13</v>
+      <c r="R2" s="24"/>
+      <c r="S2" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="T2" s="23"/>
       <c r="U2" s="23"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="22" t="s">
-        <v>11</v>
+      <c r="V2" s="23"/>
+      <c r="W2" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="X2" s="23"/>
       <c r="Y2" s="23"/>
@@ -748,60 +738,48 @@
       <c r="AF2" s="23"/>
       <c r="AG2" s="23"/>
       <c r="AH2" s="24"/>
-      <c r="AI2" s="23" t="s">
+      <c r="AI2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="27" t="s">
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="24"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="15"/>
       <c r="AQ2" s="14" t="s">
         <v>18</v>
       </c>
       <c r="AR2" s="14"/>
       <c r="AS2" s="14"/>
-      <c r="AT2" s="14"/>
-      <c r="AU2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AV2" s="14"/>
-      <c r="AW2" s="14"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="AZ2" s="14"/>
-      <c r="BA2" s="14"/>
-      <c r="BB2" s="15"/>
+      <c r="AT2" s="15"/>
     </row>
-    <row r="3" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="20"/>
-      <c r="C3" s="28"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="28"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="25"/>
       <c r="M3" s="25"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="28"/>
       <c r="P3" s="25"/>
       <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="28"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="25"/>
       <c r="T3" s="25"/>
       <c r="U3" s="25"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="28"/>
       <c r="X3" s="25"/>
       <c r="Y3" s="25"/>
       <c r="Z3" s="26"/>
@@ -813,30 +791,22 @@
       <c r="AF3" s="25"/>
       <c r="AG3" s="25"/>
       <c r="AH3" s="26"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="26"/>
+      <c r="AI3" s="17"/>
+      <c r="AJ3" s="17"/>
+      <c r="AK3" s="17"/>
+      <c r="AL3" s="17"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="17"/>
+      <c r="AO3" s="17"/>
+      <c r="AP3" s="18"/>
       <c r="AQ3" s="17"/>
       <c r="AR3" s="17"/>
       <c r="AS3" s="17"/>
-      <c r="AT3" s="17"/>
-      <c r="AU3" s="16"/>
-      <c r="AV3" s="17"/>
-      <c r="AW3" s="17"/>
-      <c r="AX3" s="18"/>
-      <c r="AY3" s="17"/>
-      <c r="AZ3" s="17"/>
-      <c r="BA3" s="17"/>
-      <c r="BB3" s="18"/>
+      <c r="AT3" s="18"/>
     </row>
-    <row r="4" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="21"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -845,10 +815,10 @@
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -857,10 +827,10 @@
       <c r="I4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -869,10 +839,10 @@
       <c r="M4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -881,10 +851,10 @@
       <c r="Q4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="T4" s="4" t="s">
@@ -893,10 +863,10 @@
       <c r="U4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="W4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="X4" s="4" t="s">
@@ -965,479 +935,407 @@
       <c r="AS4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AT4" s="4" t="s">
+      <c r="AT4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AU4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AV4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AW4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AX4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="BA4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB4" s="5" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="5" spans="2:54" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT5" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:46" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AP5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AR5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AS5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AZ5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="BA5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="BB5" s="8" t="s">
-        <v>21</v>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT6" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:54" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="V6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AO6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AP6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AR6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AS6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AZ6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="BA6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="BB6" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:54" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>21</v>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Y7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Z7" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AA7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AD7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AE7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AF7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AG7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AP7" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="AI7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP7" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="AQ7" s="9" t="s">
         <v>9</v>
@@ -1448,157 +1346,133 @@
       <c r="AS7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AT7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AU7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AW7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="BB7" s="11" t="s">
+      <c r="AT7" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:54" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>21</v>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="V8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Y8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AA8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AB8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AD8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AE8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AF8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AG8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AP8" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="AI8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP8" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="AQ8" s="9" t="s">
         <v>9</v>
@@ -1609,222 +1483,172 @@
       <c r="AS8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AT8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AU8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AW8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="BB8" s="11" t="s">
+      <c r="AT8" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="V9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="W9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AF9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AG9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AI9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AJ9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AK9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AL9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AM9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AN9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AO9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AP9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AQ9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AR9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AS9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AZ9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="BA9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="BB9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="AT9" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:54" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:54" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B12" s="12"/>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="AU2:AX3"/>
-    <mergeCell ref="AY2:BB3"/>
+  <mergeCells count="12">
+    <mergeCell ref="AM2:AP3"/>
+    <mergeCell ref="AQ2:AT3"/>
     <mergeCell ref="B2:B4"/>
+    <mergeCell ref="S2:V3"/>
     <mergeCell ref="W2:Z3"/>
     <mergeCell ref="AA2:AD3"/>
     <mergeCell ref="AE2:AH3"/>
     <mergeCell ref="AI2:AL3"/>
-    <mergeCell ref="AM2:AP3"/>
-    <mergeCell ref="AQ2:AT3"/>
     <mergeCell ref="C2:F3"/>
     <mergeCell ref="G2:J3"/>
     <mergeCell ref="K2:N3"/>
     <mergeCell ref="O2:R3"/>
-    <mergeCell ref="S2:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>